<commit_message>
- Changed nomenclature from "species" to "substances" in flow, phase and table classes - many comments, additions and minor changes in table class - Updated Matter.xlsx to reflect changes in code
</commit_message>
<xml_diff>
--- a/core/+matter/Matter.xlsx
+++ b/core/+matter/Matter.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="DieseArbeitsmappe" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Gitlab\core\+matter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STEPS Gitlab\core\+matter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="252"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="627" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="20" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="390">
   <si>
     <t>Molar mass</t>
   </si>
@@ -1196,39 +1196,7 @@
     <t>alternate name, like water for H2O</t>
   </si>
   <si>
-    <t>number of constants is not limited, as long as they written here in a new column</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">variablename of constant1, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>NEEDED!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">value of constant1, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>NEEDED!</t>
-    </r>
-  </si>
-  <si>
     <t>formation of first 7 rows is strict</t>
-  </si>
-  <si>
-    <t>complete empty rows are not allowed!</t>
   </si>
   <si>
     <t>dimension</t>
@@ -1274,49 +1242,16 @@
     <t>worksheet has to divided into individual worksheets</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Name of property, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>NEEDED!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">variablename of property, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>NEEDED!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">value of property, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>NEEDED!</t>
-    </r>
-  </si>
-  <si>
     <t>values of properties is not limited (Excel 2013 allows ‎1.048.576 ‎rows)</t>
   </si>
   <si>
-    <t>number of properties is not limited, as long as they written here in a new column (Excel 2013 allows ‎16.384 ‎columns)</t>
+    <t>Speciesname (as chemical equation)</t>
+  </si>
+  <si>
+    <t>number of constants is not limited, as long as they are written here into a new column</t>
+  </si>
+  <si>
+    <t>number of properties is not limited, as long as they are written here into a new column (Excel 2013 allows ‎16.384 ‎columns)</t>
   </si>
   <si>
     <r>
@@ -1329,11 +1264,106 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NEEDED!</t>
+      <t>REQUIRED!</t>
     </r>
   </si>
   <si>
-    <t>Speciesname (as chemical equation)</t>
+    <r>
+      <t xml:space="preserve">variablename of constant1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>REQUIRED!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">value of constant1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>REQUIRED!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Name of property, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> REQUIRED!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">variablename of property, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> REQUIRED!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">value of property, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> REQUIRED!</t>
+    </r>
+  </si>
+  <si>
+    <t>completely empty rows are not allowed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boxed area is a sample for the compound </t>
+  </si>
+  <si>
+    <t>Hydrogen Sulfate</t>
+  </si>
+  <si>
+    <t>Ozone</t>
+  </si>
+  <si>
+    <t>Nitrate</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>Carbon Dioxide</t>
+  </si>
+  <si>
+    <t>Carbon Monoxide</t>
+  </si>
+  <si>
+    <t>Hydrogen Peroxide</t>
+  </si>
+  <si>
+    <t>Potassium Superoxide</t>
+  </si>
+  <si>
+    <t>Potassium Hydroxide</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1571,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1561,6 +1591,86 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1615,7 +1725,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1722,6 +1832,18 @@
     </xf>
     <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="20% - Akzent1" xfId="1"/>
@@ -2205,110 +2327,134 @@
   <sheetPr codeName="Tabelle1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="60" t="s">
+        <v>370</v>
+      </c>
+      <c r="B1" s="61" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1" s="62"/>
+      <c r="D1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="63" t="s">
+        <v>352</v>
+      </c>
+      <c r="B2" s="64"/>
+      <c r="C2" s="65"/>
+      <c r="D2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="63" t="s">
+        <v>354</v>
+      </c>
+      <c r="B3" s="64"/>
+      <c r="C3" s="65"/>
+      <c r="D3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="63"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="65"/>
+      <c r="D4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>376</v>
+      </c>
+      <c r="E5" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="66" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="66"/>
+      <c r="B7" s="67" t="s">
+        <v>340</v>
+      </c>
+      <c r="C7" s="68" t="s">
+        <v>341</v>
+      </c>
+      <c r="D7" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="69">
+        <v>0</v>
+      </c>
+      <c r="B8" s="70">
+        <v>273.14999999999998</v>
+      </c>
+      <c r="C8" s="71">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E8" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="52" t="s">
         <v>379</v>
       </c>
-      <c r="B1" t="s">
-        <v>353</v>
-      </c>
-      <c r="D1" t="s">
-        <v>378</v>
-      </c>
-      <c r="E1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>352</v>
-      </c>
-      <c r="D2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>357</v>
-      </c>
-      <c r="D3" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>373</v>
-      </c>
-      <c r="E5" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="D7" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="52" t="s">
-        <v>358</v>
-      </c>
-      <c r="D8" t="s">
-        <v>375</v>
-      </c>
-      <c r="E8" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="53" t="str">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="53" t="str">
         <f>HYPERLINK("#'H2O'!A1","for an example refer worksheet H2O")</f>
         <v>for an example refer worksheet H2O</v>
       </c>
@@ -7680,7 +7826,7 @@
     </row>
     <row r="2" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="56" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -7761,7 +7907,7 @@
         <v>332</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -8002,7 +8148,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B1" s="17">
         <v>14541</v>
@@ -8013,7 +8159,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D2" s="1"/>
       <c r="J2" s="13"/>
@@ -8088,7 +8234,7 @@
         <v>332</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -9193,7 +9339,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="52" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -9216,9 +9362,9 @@
   </sheetPr>
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9293,14 +9439,16 @@
         <v>337</v>
       </c>
       <c r="K2" s="46" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="23" t="s">
+        <v>384</v>
+      </c>
       <c r="C3" s="19" t="s">
         <v>326</v>
       </c>
@@ -9316,7 +9464,9 @@
       <c r="G3" s="25">
         <v>0.73</v>
       </c>
-      <c r="H3" s="25"/>
+      <c r="H3" s="25">
+        <v>2165</v>
+      </c>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
     </row>
@@ -9324,7 +9474,9 @@
       <c r="A4" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="23" t="s">
+        <v>385</v>
+      </c>
       <c r="C4" s="19" t="s">
         <v>326</v>
       </c>
@@ -9350,7 +9502,9 @@
       <c r="A5" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="23" t="s">
+        <v>385</v>
+      </c>
       <c r="C5" s="19" t="s">
         <v>328</v>
       </c>
@@ -9374,7 +9528,9 @@
       <c r="A6" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="23"/>
+      <c r="B6" s="23" t="s">
+        <v>381</v>
+      </c>
       <c r="C6" s="19" t="s">
         <v>326</v>
       </c>
@@ -9396,7 +9552,9 @@
       <c r="A7" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="23" t="s">
+        <v>386</v>
+      </c>
       <c r="C7" s="19" t="s">
         <v>326</v>
       </c>
@@ -9422,7 +9580,9 @@
       <c r="A8" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="23" t="s">
+        <v>383</v>
+      </c>
       <c r="C8" s="19" t="s">
         <v>327</v>
       </c>
@@ -9440,7 +9600,9 @@
       <c r="A9" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="23" t="s">
+        <v>36</v>
+      </c>
       <c r="C9" s="19" t="s">
         <v>328</v>
       </c>
@@ -9458,7 +9620,9 @@
       <c r="A10" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="23"/>
+      <c r="B10" s="23" t="s">
+        <v>363</v>
+      </c>
       <c r="C10" s="19" t="s">
         <v>326</v>
       </c>
@@ -9484,7 +9648,9 @@
       <c r="A11" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="23"/>
+      <c r="B11" s="23" t="s">
+        <v>38</v>
+      </c>
       <c r="C11" s="19" t="s">
         <v>327</v>
       </c>
@@ -9505,7 +9671,9 @@
       <c r="A12" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="23"/>
+      <c r="B12" s="23" t="s">
+        <v>39</v>
+      </c>
       <c r="C12" s="19" t="s">
         <v>327</v>
       </c>
@@ -9524,7 +9692,9 @@
       <c r="A13" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="23"/>
+      <c r="B13" s="23" t="s">
+        <v>387</v>
+      </c>
       <c r="C13" s="19" t="s">
         <v>326</v>
       </c>
@@ -9548,7 +9718,9 @@
       <c r="A14" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="23" t="s">
+        <v>382</v>
+      </c>
       <c r="C14" s="19" t="s">
         <v>326</v>
       </c>
@@ -9572,7 +9744,9 @@
       <c r="A15" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="23" t="s">
+        <v>107</v>
+      </c>
       <c r="C15" s="19" t="s">
         <v>326</v>
       </c>
@@ -9601,7 +9775,9 @@
       <c r="A16" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="23" t="s">
+        <v>107</v>
+      </c>
       <c r="C16" s="19" t="s">
         <v>328</v>
       </c>
@@ -9622,7 +9798,9 @@
       <c r="A17" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="23" t="s">
+        <v>122</v>
+      </c>
       <c r="C17" s="19" t="s">
         <v>326</v>
       </c>
@@ -9649,7 +9827,9 @@
       <c r="A18" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="23" t="s">
+        <v>122</v>
+      </c>
       <c r="C18" s="19" t="s">
         <v>328</v>
       </c>
@@ -9676,7 +9856,9 @@
       <c r="A19" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="23" t="s">
+        <v>120</v>
+      </c>
       <c r="C19" s="19" t="s">
         <v>326</v>
       </c>
@@ -9700,7 +9882,9 @@
       <c r="A20" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="23"/>
+      <c r="B20" s="23" t="s">
+        <v>120</v>
+      </c>
       <c r="C20" s="19" t="s">
         <v>328</v>
       </c>
@@ -9724,7 +9908,9 @@
       <c r="A21" s="39" t="s">
         <v>338</v>
       </c>
-      <c r="B21" s="23"/>
+      <c r="B21" s="23" t="s">
+        <v>388</v>
+      </c>
       <c r="C21" s="19" t="s">
         <v>327</v>
       </c>
@@ -9747,7 +9933,9 @@
       <c r="A22" s="39" t="s">
         <v>339</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="23" t="s">
+        <v>389</v>
+      </c>
       <c r="C22" s="19" t="s">
         <v>328</v>
       </c>
@@ -9767,7 +9955,9 @@
       <c r="A23" s="39" t="s">
         <v>339</v>
       </c>
-      <c r="B23" s="23"/>
+      <c r="B23" s="23" t="s">
+        <v>389</v>
+      </c>
       <c r="C23" s="19" t="s">
         <v>327</v>
       </c>
@@ -12989,7 +13179,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29835,7 +30025,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B2" s="54"/>
       <c r="D2" s="1" t="s">
@@ -29960,7 +30150,7 @@
         <v>342</v>
       </c>
       <c r="F7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>343</v>
@@ -29975,7 +30165,7 @@
         <v>332</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -30912,7 +31102,7 @@
         <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -30926,7 +31116,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -31028,7 +31218,7 @@
         <v>342</v>
       </c>
       <c r="F7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>343</v>
@@ -31152,7 +31342,7 @@
         <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -31166,7 +31356,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -31271,7 +31461,7 @@
         <v>342</v>
       </c>
       <c r="F7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>343</v>
@@ -31395,7 +31585,7 @@
         <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -31409,7 +31599,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -31514,7 +31704,7 @@
         <v>342</v>
       </c>
       <c r="F7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>343</v>
@@ -31638,7 +31828,7 @@
         <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -31652,7 +31842,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -31757,7 +31947,7 @@
         <v>342</v>
       </c>
       <c r="F7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>343</v>
@@ -31926,7 +32116,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31950,7 +32140,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -32055,7 +32245,7 @@
         <v>342</v>
       </c>
       <c r="F7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>343</v>

</xml_diff>